<commit_message>
Begin aligning with new resource
</commit_message>
<xml_diff>
--- a/Join two lists of answers together and repeat over them example.xlsx
+++ b/Join two lists of answers together and repeat over them example.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexThomson\Dropbox (SSD)\TPP Questionnaire ODK\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stats4sd-my.sharepoint.com/personal/alex_thomson_stats4sd_org/Documents/ODK Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECED435F-74ED-4F6D-B31C-43556F6B3CB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -558,10 +558,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,9 +859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E7D873-2746-405F-A900-76854FB243C9}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1433,7 @@
       </c>
       <c r="D2" s="6" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2103161721</v>
+        <v>2104301328</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>

</xml_diff>